<commit_message>
Updated template to match docs
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Template.xlsx
+++ b/docs/data_providers/data_format/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorme/Research/SAFE/Database/Data_Formatting/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114AF5C5-937D-4845-B2D7-4232F1078E1C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B280D6-BD4D-1C47-A6A8-D7C1446EDC12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
-  <si>
-    <t>SAFE Project ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Access status</t>
   </si>
@@ -175,6 +172,21 @@
   </si>
   <si>
     <t>West</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Access conditions</t>
+  </si>
+  <si>
+    <t>Permit type</t>
+  </si>
+  <si>
+    <t>Permit authority</t>
+  </si>
+  <si>
+    <t>Permit number</t>
   </si>
 </sst>
 </file>
@@ -588,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A27"/>
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +613,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -616,122 +628,142 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -759,19 +791,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -801,25 +833,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -849,52 +881,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added NCBITaxa sheet to template
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Template.xlsx
+++ b/docs/data_providers/data_format/Template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B280D6-BD4D-1C47-A6A8-D7C1446EDC12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E22AD79-31F6-FE42-B165-B2310B5F0F60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Locations" sheetId="2" r:id="rId2"/>
-    <sheet name="Taxa" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
+    <sheet name="GBIFTaxa" sheetId="3" r:id="rId3"/>
+    <sheet name="NCBITaxa" sheetId="5" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Access status</t>
   </si>
@@ -187,6 +188,15 @@
   </si>
   <si>
     <t>Permit number</t>
+  </si>
+  <si>
+    <t>NCBI ID</t>
+  </si>
+  <si>
+    <t>Add taxonomic ranks here</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -602,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
@@ -821,7 +831,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,6 +879,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4E37A1-7EFA-454D-B05D-B6D6F2D27E6F}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A1030"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated template to use new NCBITaxa sheet format
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Template.xlsx
+++ b/docs/data_providers/data_format/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E22AD79-31F6-FE42-B165-B2310B5F0F60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F2E0CB-3E3D-554F-B23D-E12581211F58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Access status</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>Permit number</t>
-  </si>
-  <si>
-    <t>NCBI ID</t>
   </si>
   <si>
     <t>Add taxonomic ranks here</t>
@@ -883,7 +880,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,13 +893,13 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>